<commit_message>
Fix issue final 1
</commit_message>
<xml_diff>
--- a/public/data/halife_products.xlsx
+++ b/public/data/halife_products.xlsx
@@ -740,12 +740,12 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>/images/product-af2d0fd8-1752511729.png</t>
+          <t>/images/product-6fe759f3-1753194718.jpg</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>/images/product-a9e9eeec-1753024799.png;/images/product-0680793c-1753024799.png</t>
+          <t>/images/product-a9e9eeec-1753024799.png;/images/product-0680793c-1753024799.png;/images/product-6aa5133d-1753184918.png</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
@@ -770,7 +770,7 @@
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>2025-07-20</t>
+          <t>2025-07-22</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">

</xml_diff>